<commit_message>
Add Function for articlePage ,BlogPage ,CartPage
</commit_message>
<xml_diff>
--- a/theme creator.xlsx
+++ b/theme creator.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="collection" sheetId="1" r:id="rId1"/>
     <sheet name="404" sheetId="2" r:id="rId2"/>
     <sheet name="article" sheetId="4" r:id="rId3"/>
+    <sheet name="Blog" sheetId="5" r:id="rId4"/>
+    <sheet name="cart" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="157">
   <si>
     <t>&lt;PRODUCTS&gt;</t>
   </si>
@@ -295,13 +297,546 @@
   </si>
   <si>
     <t>&lt;/ARTICLE_FORM_COMMENT&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;ARTICLE_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;BLOGS&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;BLOG_URL&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;BLOG_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;BLOG_IMAGE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;BLOG_PUBLISED_AT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;BLOG_CONTENT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;BLOG_PAGINATE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/BLOG_PAGINATE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>blog title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for loop for blogs </t>
+  </si>
+  <si>
+    <t>vlog url</t>
+  </si>
+  <si>
+    <t>blig img url</t>
+  </si>
+  <si>
+    <t>blog publised date time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blog content </t>
+  </si>
+  <si>
+    <t>blog paginated</t>
+  </si>
+  <si>
+    <t>blog end pagination</t>
+  </si>
+  <si>
+    <t>&lt;/BLOGS&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_LABEL_PRODUCT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_LABEL_PRICE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_LABEL_QUANTITY&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CART_ITEMS&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEM_URL&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEM_IMAGE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEM_VARIANT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_PRODUCT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEM_VENDOR&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEM_PRICE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEM_KEY&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEM_QUANTITY&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEM_LINE_PRICE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEM_DESCOUNT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEMS_FOR_LOOP_INDEX&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_NOT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEMS_TOTAL_COUNT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_ITEMS_TOTAL_PRICE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_UPTADE_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_EMPTY_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>&lt;/CART_CONTINUE_HTML&gt;</t>
+  </si>
+  <si>
+    <t>cart page title</t>
+  </si>
+  <si>
+    <t>cart lable prduct</t>
+  </si>
+  <si>
+    <t>cart lable price</t>
+  </si>
+  <si>
+    <t>cart lable quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for loop for </t>
+  </si>
+  <si>
+    <t>item in cart url product page</t>
+  </si>
+  <si>
+    <t>image for product in cart</t>
+  </si>
+  <si>
+    <t>item variant title</t>
+  </si>
+  <si>
+    <t>item product title</t>
+  </si>
+  <si>
+    <t>item vendor title</t>
+  </si>
+  <si>
+    <t>item price</t>
+  </si>
+  <si>
+    <t>item key (fo delete and updte)</t>
+  </si>
+  <si>
+    <t>quantity of item</t>
+  </si>
+  <si>
+    <t>total price of this product</t>
+  </si>
+  <si>
+    <t>title descount</t>
+  </si>
+  <si>
+    <t>index for loop cart items</t>
+  </si>
+  <si>
+    <t>cart description</t>
+  </si>
+  <si>
+    <t>cart total count</t>
+  </si>
+  <si>
+    <t>cart total price</t>
+  </si>
+  <si>
+    <t>title for update cart</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CART_CHECKOUT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>cart checkout title</t>
+  </si>
+  <si>
+    <t>cart empty title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cart continue html </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,19 +850,46 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF6A8759"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -337,12 +899,21 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -365,43 +936,90 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -706,162 +1324,162 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="62.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -873,51 +1491,51 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:2" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="12" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -974,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +1603,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B1" t="s">
@@ -993,7 +1611,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B2" t="s">
@@ -1001,7 +1619,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B3" t="s">
@@ -1009,7 +1627,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B4" t="s">
@@ -1017,127 +1635,438 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="17" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+    <row r="19" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="9" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" t="s">
+        <v>156</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add function Customer Account
</commit_message>
<xml_diff>
--- a/theme creator.xlsx
+++ b/theme creator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="collection" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="article" sheetId="4" r:id="rId3"/>
     <sheet name="Blog" sheetId="5" r:id="rId4"/>
     <sheet name="cart" sheetId="6" r:id="rId5"/>
+    <sheet name="customer_account" sheetId="7" r:id="rId6"/>
+    <sheet name="customerActiveAccount" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="225">
   <si>
     <t>&lt;PRODUCTS&gt;</t>
   </si>
@@ -830,6 +832,573 @@
   </si>
   <si>
     <t xml:space="preserve">cart continue html </t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACCOUNT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACCOUNT_ORDER_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACCOUNT_FULFILLMENT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACCOUNT_PAYMENT_STATUS_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACCOUNT_ORDER_TOTAL_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ORDERS&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ORDER_NAME&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ORDER_CREATE_AT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ORDER_FINANCIAL_STATUS&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ORDER_FULFILLMENT_STATUS&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ORDER_TOTAL_PRICE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ORDER_NONE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ORDER_PAGINATION&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ORDER_PAGINATION_LIST&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ORDER_PAGINATION&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_NAME&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_EMAIL&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_DEFAULT_ADDRESS1&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_DEFAULT_ADDRESS2&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_DEFAULT_ADDRESS_CITY&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_DEFAULT_ADDRESS_PROVINCE_CODE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_DEFAULT_ADDRESS_ZIP&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_DEFAULT_ADDRESS_COUNTRY&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_DEFAULT_ADDRESS_PHONE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>&lt;/CUSTOMER_ACCOUNT_ADDRESS_PAGE&gt;</t>
+  </si>
+  <si>
+    <t>Customer Acunt Title</t>
+  </si>
+  <si>
+    <t>Customer Acunt Order title</t>
+  </si>
+  <si>
+    <t>customer paument status</t>
+  </si>
+  <si>
+    <t>customer account fulfillment title</t>
+  </si>
+  <si>
+    <t>customer account order total title</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>customer order name</t>
+  </si>
+  <si>
+    <t>customer order create at</t>
+  </si>
+  <si>
+    <t>customer order financial status</t>
+  </si>
+  <si>
+    <t>customer order fulfillment status</t>
+  </si>
+  <si>
+    <t>customer order total price</t>
+  </si>
+  <si>
+    <t>customer order none</t>
+  </si>
+  <si>
+    <t>customer order pagination</t>
+  </si>
+  <si>
+    <t>customer order pagination list</t>
+  </si>
+  <si>
+    <t>customer default address1</t>
+  </si>
+  <si>
+    <t>customer default address2</t>
+  </si>
+  <si>
+    <t>customer default address city</t>
+  </si>
+  <si>
+    <t>customer default address province code</t>
+  </si>
+  <si>
+    <t>customer default address zip</t>
+  </si>
+  <si>
+    <t>customer default address country</t>
+  </si>
+  <si>
+    <t>customer default address phone</t>
+  </si>
+  <si>
+    <t>customer account address page</t>
+  </si>
+  <si>
+    <t>customer name</t>
+  </si>
+  <si>
+    <t>customer email</t>
+  </si>
+  <si>
+    <t>customer order pagination start</t>
+  </si>
+  <si>
+    <t>&lt;/CUSTOMER_ORDERS&gt;</t>
+  </si>
+  <si>
+    <t>end for loop for orders</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACTIVE_ACCOUNT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACTIVE_ACCOUNT_SUBTEXT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ACTIVE_ACCOUNT_FORM&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACTIVE_ACCOUNT_PASSWORD_TEXT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACTIVE_ACCOUNT_PASSWORD_CONFIRM_TEXT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACTIVE_ACCOUNT_SUBMIT_TEXT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACTIVE_ACCOUNT_CANCEL_TEXT&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACTIVE_ACCOUNT_ERROR&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ACTIVE_ACCOUNT_FORM&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>customer active accont title</t>
+  </si>
+  <si>
+    <t>customer active accont subtext</t>
+  </si>
+  <si>
+    <t>customer active accont error</t>
+  </si>
+  <si>
+    <t>start customer active accont form</t>
+  </si>
+  <si>
+    <t>end customer active accont form</t>
+  </si>
+  <si>
+    <t>customer active account accont text in form</t>
+  </si>
+  <si>
+    <t>customer active account password accont text in form</t>
   </si>
 </sst>
 </file>
@@ -1866,8 +2435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2071,4 +2640,323 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B23" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B24" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="79" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add function  customer_address ,customer_activ_account ,customer_login ,customer_order
</commit_message>
<xml_diff>
--- a/theme creator.xlsx
+++ b/theme creator.xlsx
@@ -14,6 +14,7 @@
     <sheet name="cart" sheetId="6" r:id="rId5"/>
     <sheet name="customer_account" sheetId="7" r:id="rId6"/>
     <sheet name="customerActiveAccount" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -2959,4 +2960,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add function collection page, page contact, customer_account, update file exel theme createor and crate folder simpl page Shopify
</commit_message>
<xml_diff>
--- a/theme creator.xlsx
+++ b/theme creator.xlsx
@@ -4,24 +4,25 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="collection" sheetId="1" r:id="rId1"/>
     <sheet name="404" sheetId="2" r:id="rId2"/>
     <sheet name="article" sheetId="4" r:id="rId3"/>
-    <sheet name="Blog" sheetId="5" r:id="rId4"/>
-    <sheet name="cart" sheetId="6" r:id="rId5"/>
+    <sheet name="cart" sheetId="6" r:id="rId4"/>
+    <sheet name="Blog" sheetId="5" r:id="rId5"/>
     <sheet name="customer_account" sheetId="7" r:id="rId6"/>
     <sheet name="customerActiveAccount" sheetId="8" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
+    <sheet name="Customer_Address" sheetId="9" r:id="rId8"/>
+    <sheet name="customer_login" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="435">
   <si>
     <t>&lt;PRODUCTS&gt;</t>
   </si>
@@ -1400,13 +1401,1380 @@
   </si>
   <si>
     <t>customer active account password accont text in form</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_LAST_NAME_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_LAST_NAME_FORM_VALUE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_COMPANY_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_COMPANY_FORM_VALUE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_ADDRESS1_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_ADDRESS1_FORM_VALUE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_ADDRESS2_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_ADDRESS2_FORM_VALUE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_CITY_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_CITY_FORM_VALUE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_COUNTRY_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_PROVINCE_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_FORM_PROVINCE_VALUE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_FORM_ID&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_ZIP&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_FORM_ZIP&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_PHONE_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_FORM_PHONE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_SET_DEFAULT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>&lt;/CUSTOMER_ADDRESS_SET_AS_DEFAULT_ADDRESS&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_ADD_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_CANCEL&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_TITLE_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ADDRESS_ADDRESSES&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>&lt;CUSTOMER_ADDRESS_ADDRESSE_EDIT&gt;\</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ADDRESS_ADDRESSE_DELETE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ADDRESS_ADDRESSE_COMPANY&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ADDRESS_ADDRESSE_STREET&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ADDRESS_ADDRESSE_CITY&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ADDRESS_ADDRESSE_PROVINCE_CODE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ADDRESS_ADDRESSE_COUNTRY&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ADDRESS_ADDRESSE_PHONE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ADDRESS_ADDRESSE_PAGINATES&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_ADDRESS_ADDRESSE_FORM&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_ACCOUNT_RETURN&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_ACCOUNT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_OPTION_TAGS&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_FORM_COUNTRY&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_EDIT_DEFAULT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_CUSTOMER_ADDRESSES&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_CUSTOMER_ADDRESS_ID&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_CUSTOMER_ADDRESS_UPDATE_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_PAGINATE_IF&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_PAGINATE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/ENDIF&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/END_FORM&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/ENDFOR&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_FORM&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_ERROR_FORM&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_ADD_NEW&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_FIRST_NAME_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_ADDRESS_FIRST_NAME_FORM_VALUE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>customer address form</t>
+  </si>
+  <si>
+    <t>customer address error form</t>
+  </si>
+  <si>
+    <t>customer address add new</t>
+  </si>
+  <si>
+    <t>customer address first name title</t>
+  </si>
+  <si>
+    <t>customer address first name form value</t>
+  </si>
+  <si>
+    <t>customer address last name title</t>
+  </si>
+  <si>
+    <t>customer address last name form value</t>
+  </si>
+  <si>
+    <t>customer address company title</t>
+  </si>
+  <si>
+    <t>customer address company form value</t>
+  </si>
+  <si>
+    <t>customer address address1 title</t>
+  </si>
+  <si>
+    <t>customer address address1 form value</t>
+  </si>
+  <si>
+    <t>customer address address2 title</t>
+  </si>
+  <si>
+    <t>customer address address2 form value</t>
+  </si>
+  <si>
+    <t>customer address city title</t>
+  </si>
+  <si>
+    <t>customer address city form value</t>
+  </si>
+  <si>
+    <t>customer address country title</t>
+  </si>
+  <si>
+    <t>customer address province title</t>
+  </si>
+  <si>
+    <t>customer address form province value</t>
+  </si>
+  <si>
+    <t>customer address form id</t>
+  </si>
+  <si>
+    <t>customer address zip</t>
+  </si>
+  <si>
+    <t>customer address form zip</t>
+  </si>
+  <si>
+    <t>customer address phone title</t>
+  </si>
+  <si>
+    <t>customer address form phone</t>
+  </si>
+  <si>
+    <t>customer address set default title</t>
+  </si>
+  <si>
+    <t>customer address set as default address</t>
+  </si>
+  <si>
+    <t>customer address add title</t>
+  </si>
+  <si>
+    <t>customer address cancel</t>
+  </si>
+  <si>
+    <t>customer address title title</t>
+  </si>
+  <si>
+    <t>customer address addresses</t>
+  </si>
+  <si>
+    <t>customer address addresse edit</t>
+  </si>
+  <si>
+    <t>customer address addresse delete</t>
+  </si>
+  <si>
+    <t>customer address addresse company</t>
+  </si>
+  <si>
+    <t>customer address addresse street</t>
+  </si>
+  <si>
+    <t>customer address addresse city</t>
+  </si>
+  <si>
+    <t>customer address addresse province code</t>
+  </si>
+  <si>
+    <t>customer address addresse country</t>
+  </si>
+  <si>
+    <t>customer address addresse phone</t>
+  </si>
+  <si>
+    <t>customer address addresse paginates</t>
+  </si>
+  <si>
+    <t>customer address addresse form</t>
+  </si>
+  <si>
+    <t>customer address account return</t>
+  </si>
+  <si>
+    <t>customer address account title</t>
+  </si>
+  <si>
+    <t>customer address option tags</t>
+  </si>
+  <si>
+    <t>customer address form country</t>
+  </si>
+  <si>
+    <t>customer address edit default title</t>
+  </si>
+  <si>
+    <t>customer address customer addresses</t>
+  </si>
+  <si>
+    <t>customer address customer address id</t>
+  </si>
+  <si>
+    <t>customer address customer address update title</t>
+  </si>
+  <si>
+    <t>customer address paginate if</t>
+  </si>
+  <si>
+    <t>customer address paginate</t>
+  </si>
+  <si>
+    <t>endif</t>
+  </si>
+  <si>
+    <t>form</t>
+  </si>
+  <si>
+    <t>endfor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ 'customer.addresses.phone' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ form.phone }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.addresses.set_default' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ form.set_as_default_checkbox }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.addresses.add' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.addresses.cancel' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.addresses.title' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% for address in customer.addresses %} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.addresses.edit' | t | edit_customer_address_link: address.id }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.addresses.delete' | t | delete_customer_address_link: address.id }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ address.company }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ address.street }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ address.city | capitalize }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% if address.province_code %}{{ address.province_code | upcase }}{% endif %} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ address.country }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ address.phone }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% paginate customer.addresses by 5 %} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% form 'customer_address', customer.new_address %} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.account.return' | t }} </t>
+  </si>
+  <si>
+    <t>{{ 'customer.account.title' | t }}</t>
+  </si>
+  <si>
+    <t>{{ country_option_tags }}</t>
+  </si>
+  <si>
+    <t>{{ form.country }}</t>
+  </si>
+  <si>
+    <t>{{ 'customer.addresses.edit_address' | t }}</t>
+  </si>
+  <si>
+    <t>{% form  'customer_address', address %}</t>
+  </si>
+  <si>
+    <t>{{ address.id }}</t>
+  </si>
+  <si>
+    <t>{{ 'customer.addresses.update' | t }}</t>
+  </si>
+  <si>
+    <t>{% if paginate.pages &gt; 1 %}</t>
+  </si>
+  <si>
+    <t>{{ paginate | default_pagination | replace: '&amp;laquo; Previous', '&amp;larr;' | replace: 'Next &amp;raquo;', '&amp;rarr;' }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% endif %}  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% endfor %} </t>
+  </si>
+  <si>
+    <t>helper page url</t>
+  </si>
+  <si>
+    <t>https://help.shopify.com/en/themes/development/templates/customers-addresses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple page </t>
+  </si>
+  <si>
+    <t>simple page Shopify\addresses.liquid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ form.errors | default_errors }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.addresses.add_new' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.addresses.first_name' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ form.first_name }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ 'customer.addresses.last_name' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ form.last_name }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.addresses.company' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ 'customer.addresses.address1' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ form.address1 }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.addresses.address2' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ form.address2 }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ 'customer.addresses.city' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ form.city }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ 'customer.addresses.country' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ 'customer.addresses.province' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ form.province }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ 'customer.addresses.zip' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ form.id }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ form.zip }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {{ form.company }} </t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_RECOVER_PASSWORD&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;CUSTOMER_LOGIN_FORM&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_ERROR&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_EMAIL_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_PASSWORD_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_FORGET_PASSWORD_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_SING_IN_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_LOGIN_CANCEL_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_CRETE_ACCOUNT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_PASSWORD_SUB_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_RECOVER_EMAIL&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_RECOVER_PASSWORD_SUBMIT_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_PASSWORD_CANCEL&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_GUST_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_GUST_CONTINUE_TITLE&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;/CUSTOMER_LOGIN_FORM&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13.5"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>customer login recover password</t>
+  </si>
+  <si>
+    <t>customer login form</t>
+  </si>
+  <si>
+    <t>customer login error</t>
+  </si>
+  <si>
+    <t>customer login title</t>
+  </si>
+  <si>
+    <t>customer login email title</t>
+  </si>
+  <si>
+    <t>customer login password title</t>
+  </si>
+  <si>
+    <t>customer login forget password title</t>
+  </si>
+  <si>
+    <t>customer login sing in title</t>
+  </si>
+  <si>
+    <t>customer login login cancel title</t>
+  </si>
+  <si>
+    <t>customer login crete account title</t>
+  </si>
+  <si>
+    <t>customer login password sub title</t>
+  </si>
+  <si>
+    <t>customer login recover email</t>
+  </si>
+  <si>
+    <t>customer login recover password submit title</t>
+  </si>
+  <si>
+    <t>customer login password cancel</t>
+  </si>
+  <si>
+    <t>customer login gust title</t>
+  </si>
+  <si>
+    <t>customer login gust continue title</t>
+  </si>
+  <si>
+    <t>{{ 'customer.recover_password.success' | t }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% form 'customer_login' %} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.login.title' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.login.email' | t }} </t>
+  </si>
+  <si>
+    <t>{{ 'customer.login.password' | t }}</t>
+  </si>
+  <si>
+    <t>{{ 'customer.login.forgot_password' | t }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.login.sign_in' | t }} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ 'customer.login.cancel' | t }} </t>
+  </si>
+  <si>
+    <t>{{ 'layout.customer.create_account' | t | customer_register_link }}</t>
+  </si>
+  <si>
+    <t>{{ 'customer.recover_password.email' | t }}</t>
+  </si>
+  <si>
+    <t>{{ 'customer.recover_password.submit' | t }}</t>
+  </si>
+  <si>
+    <t>{{ 'customer.recover_password.cancel' | t }}</t>
+  </si>
+  <si>
+    <t>{{ 'customer.login.guest_continue' | t }}</t>
+  </si>
+  <si>
+    <t>{% endform %}</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>{{ 'customer.recover_password.subtext' | t }},</t>
+  </si>
+  <si>
+    <t>https://help.shopify.com/en/themes/development/templates/customers-login</t>
+  </si>
+  <si>
+    <t>simple page</t>
+  </si>
+  <si>
+    <t>simple page Shopify\login.liquid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1453,8 +2821,32 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1482,8 +2874,13 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1532,14 +2929,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1584,12 +3014,30 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="5"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="5" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="4" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="4"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="7">
+    <cellStyle name="Calculation" xfId="5" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
+    <cellStyle name="Output" xfId="4" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2334,6 +3782,217 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B24" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2429,217 +4088,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B24" t="s">
-        <v>156</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2875,7 +4323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2964,12 +4412,857 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="B4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="B7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B10" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B12" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" t="s">
+        <v>289</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B14" t="s">
+        <v>290</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" t="s">
+        <v>291</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B16" t="s">
+        <v>292</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B17" t="s">
+        <v>293</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18" t="s">
+        <v>294</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" t="s">
+        <v>295</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B20" t="s">
+        <v>296</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" t="s">
+        <v>297</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B22" t="s">
+        <v>298</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="D22" s="21"/>
+    </row>
+    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" t="s">
+        <v>299</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B24" t="s">
+        <v>300</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="B25" t="s">
+        <v>301</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26" t="s">
+        <v>302</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B27" t="s">
+        <v>303</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B28" t="s">
+        <v>304</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B29" t="s">
+        <v>305</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B30" t="s">
+        <v>306</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B31" t="s">
+        <v>307</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="B32" t="s">
+        <v>308</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B33" t="s">
+        <v>309</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B34" t="s">
+        <v>310</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B35" t="s">
+        <v>311</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B36" t="s">
+        <v>312</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="B37" t="s">
+        <v>313</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B38" t="s">
+        <v>314</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="B39" t="s">
+        <v>315</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B40" t="s">
+        <v>316</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="B41" t="s">
+        <v>317</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B42" t="s">
+        <v>318</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B43" t="s">
+        <v>319</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B44" t="s">
+        <v>320</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="B45" t="s">
+        <v>321</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B46" t="s">
+        <v>322</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B47" t="s">
+        <v>323</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B48" t="s">
+        <v>322</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B49" t="s">
+        <v>324</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B50" t="s">
+        <v>325</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B51" t="s">
+        <v>326</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B52" t="s">
+        <v>327</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B53" t="s">
+        <v>328</v>
+      </c>
+      <c r="C53" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>359</v>
+      </c>
+      <c r="B57" s="27" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>361</v>
+      </c>
+      <c r="B58" s="27" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B57" r:id="rId1"/>
+    <hyperlink ref="B58" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="77.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="188.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="B1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="B2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B4" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="B5" t="s">
+        <v>404</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="B6" t="s">
+        <v>405</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="B7" t="s">
+        <v>406</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="B8" t="s">
+        <v>407</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="B9" t="s">
+        <v>408</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="B10" t="s">
+        <v>409</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="B11" t="s">
+        <v>410</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="B12" t="s">
+        <v>411</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="B13" t="s">
+        <v>412</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="B14" t="s">
+        <v>413</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="B15" t="s">
+        <v>414</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="B16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="B17" t="s">
+        <v>401</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="23"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>359</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>433</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C20" r:id="rId1"/>
+    <hyperlink ref="C21" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add graphql in project
</commit_message>
<xml_diff>
--- a/theme creator.xlsx
+++ b/theme creator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="557" firstSheet="12" activeTab="14"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="557"/>
   </bookViews>
   <sheets>
     <sheet name="collectionPage" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="1009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="1012">
   <si>
     <t>start loop for all product</t>
   </si>
@@ -2490,36 +2490,6 @@
     <t>{{-CUSTOMER_ADDRESS_ADDRESSES}}</t>
   </si>
   <si>
-    <t>{{-CUSTOMER_ADDRESS_ADDRESSE_EDIT}}\</t>
-  </si>
-  <si>
-    <t>{{-CUSTOMER_ADDRESS_ADDRESSE_DELETE}}</t>
-  </si>
-  <si>
-    <t>{{-CUSTOMER_ADDRESS_ADDRESSE_COMPANY}}</t>
-  </si>
-  <si>
-    <t>{{-CUSTOMER_ADDRESS_ADDRESSE_STREET}}</t>
-  </si>
-  <si>
-    <t>{{-CUSTOMER_ADDRESS_ADDRESSE_CITY}}</t>
-  </si>
-  <si>
-    <t>{{-CUSTOMER_ADDRESS_ADDRESSE_PROVINCE_CODE}}</t>
-  </si>
-  <si>
-    <t>{{-CUSTOMER_ADDRESS_ADDRESSE_COUNTRY}}</t>
-  </si>
-  <si>
-    <t>{{-CUSTOMER_ADDRESS_ADDRESSE_PHONE}}</t>
-  </si>
-  <si>
-    <t>{{-CUSTOMER_ADDRESS_ADDRESSE_PAGINATES}}</t>
-  </si>
-  <si>
-    <t>{{-CUSTOMER_ADDRESS_ADDRESSE_FORM}}</t>
-  </si>
-  <si>
     <t>{{CUSTOMER_ADDRESS_ACCOUNT_RETURN}}</t>
   </si>
   <si>
@@ -3067,6 +3037,45 @@
   </si>
   <si>
     <t xml:space="preserve">{{-PAGE_SEARCH_RESULT}} </t>
+  </si>
+  <si>
+    <t>{{-CUSTOMER_ADDRESS_ADDRESS_DELETE}}</t>
+  </si>
+  <si>
+    <t>{{-CUSTOMER_ADDRESS_ADDRESS_COMPANY}}</t>
+  </si>
+  <si>
+    <t>{{-CUSTOMER_ADDRESS_ADDRESS_STREET}}</t>
+  </si>
+  <si>
+    <t>{{-CUSTOMER_ADDRESS_ADDRESS_CITY}}</t>
+  </si>
+  <si>
+    <t>{{-CUSTOMER_ADDRESS_ADDRESS_PROVINCE_CODE}}</t>
+  </si>
+  <si>
+    <t>{{-CUSTOMER_ADDRESS_ADDRESS_COUNTRY}}</t>
+  </si>
+  <si>
+    <t>{{-CUSTOMER_ADDRESS_ADDRESS_PHONE}}</t>
+  </si>
+  <si>
+    <t>{{-CUSTOMER_ADDRESS_ADDRESS_PAGINATES}}</t>
+  </si>
+  <si>
+    <t>{{-CUSTOMER_ADDRESS_ADDRESS_FORM}}</t>
+  </si>
+  <si>
+    <t>{{-CUSTOMER_ADDRESS_ADDRESS_EDIT}}\</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {% if product.metafields.images.all %}{% assign images = product.metafields.images.all | split: " | reverse  %}{% assign image = images[0] | split: jpg" %}{{image}}_S.jpg  {%else%}{{ product.featured_image | product_img_url: "medium" }}{% endif %}'</t>
+  </si>
+  <si>
+    <t>{{PRODUCT_IMG_URL}}</t>
+  </si>
+  <si>
+    <t>{% if product.metafields.images.all %}{% assign images = product.metafields.images.all | split: " | reverse  %}{% assign image = images[0] | split: jpg" %}{{image}}_S.jpg  {%else%}{{ product.featured_image | product_img_url: "medium" }}{% endif %}</t>
   </si>
 </sst>
 </file>
@@ -3262,7 +3271,7 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3332,6 +3341,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
@@ -3645,8 +3657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4326,6 +4338,22 @@
         <v>561</v>
       </c>
     </row>
+    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="D25" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="26" spans="1:53" ht="18" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>1011</v>
+      </c>
+    </row>
     <row r="27" spans="1:53" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="24" t="s">
         <v>562</v>
@@ -4360,7 +4388,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>854</v>
+        <v>844</v>
       </c>
       <c r="B1" t="s">
         <v>357</v>
@@ -4371,7 +4399,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>855</v>
+        <v>845</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>367</v>
@@ -4382,7 +4410,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="B3" t="s">
         <v>359</v>
@@ -4393,7 +4421,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>857</v>
+        <v>847</v>
       </c>
       <c r="B4" t="s">
         <v>360</v>
@@ -4404,7 +4432,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>858</v>
+        <v>848</v>
       </c>
       <c r="B5" t="s">
         <v>361</v>
@@ -4415,7 +4443,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>859</v>
+        <v>849</v>
       </c>
       <c r="B6" t="s">
         <v>362</v>
@@ -4426,7 +4454,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>860</v>
+        <v>850</v>
       </c>
       <c r="B7" t="s">
         <v>363</v>
@@ -4437,7 +4465,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>861</v>
+        <v>851</v>
       </c>
       <c r="B8" t="s">
         <v>364</v>
@@ -4448,7 +4476,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>862</v>
+        <v>852</v>
       </c>
       <c r="B9" t="s">
         <v>365</v>
@@ -4459,7 +4487,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>863</v>
+        <v>853</v>
       </c>
       <c r="B10" t="s">
         <v>366</v>
@@ -4470,7 +4498,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>864</v>
+        <v>854</v>
       </c>
       <c r="B11" t="s">
         <v>244</v>
@@ -4481,7 +4509,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>865</v>
+        <v>855</v>
       </c>
       <c r="B12" t="s">
         <v>243</v>
@@ -4492,7 +4520,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>866</v>
+        <v>856</v>
       </c>
       <c r="B13" t="s">
         <v>245</v>
@@ -4514,7 +4542,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>867</v>
+        <v>857</v>
       </c>
       <c r="B15" t="s">
         <v>247</v>
@@ -4525,7 +4553,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>868</v>
+        <v>858</v>
       </c>
       <c r="B16" t="s">
         <v>248</v>
@@ -4536,7 +4564,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>869</v>
+        <v>859</v>
       </c>
       <c r="B17" t="s">
         <v>249</v>
@@ -4547,7 +4575,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>870</v>
+        <v>860</v>
       </c>
       <c r="B18" t="s">
         <v>250</v>
@@ -4558,7 +4586,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>871</v>
+        <v>861</v>
       </c>
       <c r="B19" t="s">
         <v>251</v>
@@ -4569,7 +4597,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>872</v>
+        <v>862</v>
       </c>
       <c r="B20" t="s">
         <v>252</v>
@@ -4580,7 +4608,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>873</v>
+        <v>863</v>
       </c>
       <c r="B21" t="s">
         <v>253</v>
@@ -4591,7 +4619,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>874</v>
+        <v>864</v>
       </c>
       <c r="B22" t="s">
         <v>254</v>
@@ -4602,7 +4630,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>875</v>
+        <v>865</v>
       </c>
       <c r="B23" t="s">
         <v>255</v>
@@ -4641,12 +4669,12 @@
         <v>256</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>876</v>
+        <v>866</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>877</v>
+        <v>867</v>
       </c>
       <c r="B27" t="s">
         <v>257</v>
@@ -4657,7 +4685,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>878</v>
+        <v>868</v>
       </c>
       <c r="B28" t="s">
         <v>258</v>
@@ -4668,7 +4696,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>879</v>
+        <v>869</v>
       </c>
       <c r="B29" t="s">
         <v>259</v>
@@ -4679,7 +4707,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>880</v>
+        <v>870</v>
       </c>
       <c r="B30" t="s">
         <v>260</v>
@@ -4690,7 +4718,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>881</v>
+        <v>871</v>
       </c>
       <c r="B31" t="s">
         <v>261</v>
@@ -4701,7 +4729,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>882</v>
+        <v>872</v>
       </c>
       <c r="B32" t="s">
         <v>262</v>
@@ -4712,7 +4740,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>883</v>
+        <v>873</v>
       </c>
       <c r="B33" t="s">
         <v>263</v>
@@ -4723,7 +4751,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>884</v>
+        <v>874</v>
       </c>
       <c r="B34" t="s">
         <v>264</v>
@@ -4734,7 +4762,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>885</v>
+        <v>875</v>
       </c>
       <c r="B35" t="s">
         <v>265</v>
@@ -4745,7 +4773,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>886</v>
+        <v>876</v>
       </c>
       <c r="B36" t="s">
         <v>266</v>
@@ -4756,7 +4784,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>887</v>
+        <v>877</v>
       </c>
       <c r="B37" t="s">
         <v>267</v>
@@ -4767,7 +4795,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>888</v>
+        <v>878</v>
       </c>
       <c r="B38" t="s">
         <v>268</v>
@@ -4778,7 +4806,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>889</v>
+        <v>879</v>
       </c>
       <c r="B39" t="s">
         <v>269</v>
@@ -4789,7 +4817,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>890</v>
+        <v>880</v>
       </c>
       <c r="B40" t="s">
         <v>270</v>
@@ -4800,7 +4828,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>891</v>
+        <v>881</v>
       </c>
       <c r="B41" t="s">
         <v>271</v>
@@ -4811,7 +4839,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>892</v>
+        <v>882</v>
       </c>
       <c r="B42" t="s">
         <v>272</v>
@@ -4822,7 +4850,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>893</v>
+        <v>883</v>
       </c>
       <c r="B43" t="s">
         <v>273</v>
@@ -4833,7 +4861,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>894</v>
+        <v>884</v>
       </c>
       <c r="B44" t="s">
         <v>274</v>
@@ -4844,7 +4872,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>895</v>
+        <v>885</v>
       </c>
       <c r="B45" t="s">
         <v>275</v>
@@ -4855,7 +4883,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>896</v>
+        <v>886</v>
       </c>
       <c r="B46" t="s">
         <v>276</v>
@@ -4866,7 +4894,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>897</v>
+        <v>887</v>
       </c>
       <c r="B47" t="s">
         <v>277</v>
@@ -4877,7 +4905,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>898</v>
+        <v>888</v>
       </c>
       <c r="B48" t="s">
         <v>278</v>
@@ -4888,7 +4916,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>899</v>
+        <v>889</v>
       </c>
       <c r="B49" t="s">
         <v>279</v>
@@ -4899,7 +4927,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="B50" t="s">
         <v>280</v>
@@ -4910,7 +4938,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>901</v>
+        <v>891</v>
       </c>
       <c r="B51" t="s">
         <v>281</v>
@@ -4921,7 +4949,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>902</v>
+        <v>892</v>
       </c>
       <c r="B52" t="s">
         <v>282</v>
@@ -4932,7 +4960,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>903</v>
+        <v>893</v>
       </c>
       <c r="B53" t="s">
         <v>283</v>
@@ -4943,7 +4971,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
       <c r="B54" t="s">
         <v>284</v>
@@ -4954,7 +4982,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>905</v>
+        <v>895</v>
       </c>
       <c r="B55" t="s">
         <v>285</v>
@@ -4965,7 +4993,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>906</v>
+        <v>896</v>
       </c>
       <c r="B56" t="s">
         <v>286</v>
@@ -4976,7 +5004,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>907</v>
+        <v>897</v>
       </c>
       <c r="B57" t="s">
         <v>287</v>
@@ -4987,7 +5015,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>908</v>
+        <v>898</v>
       </c>
       <c r="B58" t="s">
         <v>288</v>
@@ -4998,7 +5026,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>909</v>
+        <v>899</v>
       </c>
       <c r="B59" t="s">
         <v>289</v>
@@ -5009,7 +5037,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>910</v>
+        <v>900</v>
       </c>
       <c r="B60" t="s">
         <v>290</v>
@@ -5020,7 +5048,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>911</v>
+        <v>901</v>
       </c>
       <c r="B61" t="s">
         <v>291</v>
@@ -5031,7 +5059,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>912</v>
+        <v>902</v>
       </c>
       <c r="B62" t="s">
         <v>292</v>
@@ -5042,7 +5070,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>913</v>
+        <v>903</v>
       </c>
       <c r="B63" t="s">
         <v>293</v>
@@ -5053,7 +5081,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>914</v>
+        <v>904</v>
       </c>
       <c r="B64" t="s">
         <v>294</v>
@@ -5064,7 +5092,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>915</v>
+        <v>905</v>
       </c>
       <c r="B65" t="s">
         <v>295</v>
@@ -5107,7 +5135,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>916</v>
+        <v>906</v>
       </c>
       <c r="B1" t="s">
         <v>370</v>
@@ -5118,7 +5146,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>917</v>
+        <v>907</v>
       </c>
       <c r="B2" t="s">
         <v>371</v>
@@ -5129,7 +5157,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>918</v>
+        <v>908</v>
       </c>
       <c r="B3" t="s">
         <v>372</v>
@@ -5140,7 +5168,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>919</v>
+        <v>909</v>
       </c>
       <c r="B4" t="s">
         <v>373</v>
@@ -5151,7 +5179,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>920</v>
+        <v>910</v>
       </c>
       <c r="B5" t="s">
         <v>374</v>
@@ -5162,7 +5190,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>921</v>
+        <v>911</v>
       </c>
       <c r="B6" t="s">
         <v>375</v>
@@ -5173,7 +5201,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>922</v>
+        <v>912</v>
       </c>
       <c r="B7" t="s">
         <v>376</v>
@@ -5184,7 +5212,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>923</v>
+        <v>913</v>
       </c>
       <c r="B8" t="s">
         <v>377</v>
@@ -5195,7 +5223,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>924</v>
+        <v>914</v>
       </c>
       <c r="B9" t="s">
         <v>378</v>
@@ -5206,7 +5234,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>925</v>
+        <v>915</v>
       </c>
       <c r="B10" t="s">
         <v>379</v>
@@ -5217,7 +5245,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>926</v>
+        <v>916</v>
       </c>
       <c r="B11" t="s">
         <v>380</v>
@@ -5228,7 +5256,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>927</v>
+        <v>917</v>
       </c>
       <c r="B12" t="s">
         <v>381</v>
@@ -5239,7 +5267,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>928</v>
+        <v>918</v>
       </c>
       <c r="B13" t="s">
         <v>382</v>
@@ -5250,7 +5278,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>929</v>
+        <v>919</v>
       </c>
       <c r="B14" t="s">
         <v>383</v>
@@ -5261,7 +5289,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>930</v>
+        <v>920</v>
       </c>
       <c r="B15" t="s">
         <v>384</v>
@@ -5272,7 +5300,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>931</v>
+        <v>921</v>
       </c>
       <c r="B16" t="s">
         <v>385</v>
@@ -5283,7 +5311,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>932</v>
+        <v>922</v>
       </c>
       <c r="B17" t="s">
         <v>386</v>
@@ -5294,7 +5322,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>933</v>
+        <v>923</v>
       </c>
       <c r="B18" t="s">
         <v>387</v>
@@ -5305,7 +5333,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>934</v>
+        <v>924</v>
       </c>
       <c r="B19" t="s">
         <v>388</v>
@@ -5316,7 +5344,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>935</v>
+        <v>925</v>
       </c>
       <c r="B20" t="s">
         <v>389</v>
@@ -5327,7 +5355,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>936</v>
+        <v>926</v>
       </c>
       <c r="B21" t="s">
         <v>390</v>
@@ -5338,7 +5366,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>937</v>
+        <v>927</v>
       </c>
       <c r="B22" t="s">
         <v>391</v>
@@ -5349,7 +5377,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>938</v>
+        <v>928</v>
       </c>
       <c r="B23" t="s">
         <v>392</v>
@@ -5360,7 +5388,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>939</v>
+        <v>929</v>
       </c>
       <c r="B24" t="s">
         <v>393</v>
@@ -5371,7 +5399,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>940</v>
+        <v>930</v>
       </c>
       <c r="B25" t="s">
         <v>394</v>
@@ -5382,7 +5410,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>941</v>
+        <v>931</v>
       </c>
       <c r="B26" t="s">
         <v>396</v>
@@ -5393,7 +5421,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>942</v>
+        <v>932</v>
       </c>
       <c r="B27" t="s">
         <v>152</v>
@@ -5404,7 +5432,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>943</v>
+        <v>933</v>
       </c>
       <c r="B28" t="s">
         <v>397</v>
@@ -5443,7 +5471,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>944</v>
+        <v>934</v>
       </c>
       <c r="B1" t="s">
         <v>426</v>
@@ -5454,7 +5482,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>945</v>
+        <v>935</v>
       </c>
       <c r="B2" t="s">
         <v>427</v>
@@ -5465,7 +5493,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>946</v>
+        <v>936</v>
       </c>
       <c r="B3" t="s">
         <v>428</v>
@@ -5476,7 +5504,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>947</v>
+        <v>937</v>
       </c>
       <c r="B4" t="s">
         <v>429</v>
@@ -5487,7 +5515,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>948</v>
+        <v>938</v>
       </c>
       <c r="B5" t="s">
         <v>430</v>
@@ -5498,7 +5526,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>949</v>
+        <v>939</v>
       </c>
       <c r="B6" t="s">
         <v>431</v>
@@ -5509,7 +5537,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>950</v>
+        <v>940</v>
       </c>
       <c r="B7" t="s">
         <v>430</v>
@@ -5571,8 +5599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5584,7 +5612,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>951</v>
+        <v>941</v>
       </c>
       <c r="B1" t="s">
         <v>439</v>
@@ -5595,7 +5623,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>952</v>
+        <v>942</v>
       </c>
       <c r="B2" t="s">
         <v>440</v>
@@ -5606,7 +5634,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>953</v>
+        <v>943</v>
       </c>
       <c r="B3" t="s">
         <v>441</v>
@@ -5617,7 +5645,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>954</v>
+        <v>944</v>
       </c>
       <c r="B4" t="s">
         <v>442</v>
@@ -5628,7 +5656,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>955</v>
+        <v>945</v>
       </c>
       <c r="B5" t="s">
         <v>443</v>
@@ -5639,7 +5667,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>956</v>
+        <v>946</v>
       </c>
       <c r="B6" t="s">
         <v>444</v>
@@ -5650,7 +5678,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>957</v>
+        <v>947</v>
       </c>
       <c r="B7" t="s">
         <v>445</v>
@@ -5661,7 +5689,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>958</v>
+        <v>948</v>
       </c>
       <c r="B8" t="s">
         <v>446</v>
@@ -5672,24 +5700,24 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>959</v>
+        <v>949</v>
       </c>
       <c r="B9" t="s">
         <v>447</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>960</v>
+        <v>950</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>961</v>
+        <v>951</v>
       </c>
       <c r="B10" t="s">
         <v>448</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>962</v>
+        <v>952</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5734,6 +5762,17 @@
       </c>
       <c r="C14" s="23" t="s">
         <v>422</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>972</v>
+      </c>
+      <c r="B15" t="s">
+        <v>495</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>1009</v>
       </c>
     </row>
     <row r="17" spans="2:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -5749,6 +5788,7 @@
     <hyperlink ref="C17" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5769,7 +5809,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>963</v>
+        <v>953</v>
       </c>
       <c r="B1" t="s">
         <v>459</v>
@@ -5780,7 +5820,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>964</v>
+        <v>954</v>
       </c>
       <c r="B2" t="s">
         <v>460</v>
@@ -5791,7 +5831,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>965</v>
+        <v>955</v>
       </c>
       <c r="B3" t="s">
         <v>461</v>
@@ -5802,7 +5842,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="B4" t="s">
         <v>462</v>
@@ -5813,7 +5853,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>967</v>
+        <v>957</v>
       </c>
       <c r="B5" t="s">
         <v>463</v>
@@ -5824,7 +5864,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>968</v>
+        <v>958</v>
       </c>
       <c r="B6" t="s">
         <v>464</v>
@@ -5835,7 +5875,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>969</v>
+        <v>959</v>
       </c>
       <c r="B7" t="s">
         <v>465</v>
@@ -5846,7 +5886,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>970</v>
+        <v>960</v>
       </c>
       <c r="B8" t="s">
         <v>466</v>
@@ -5857,7 +5897,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>971</v>
+        <v>961</v>
       </c>
       <c r="B9" t="s">
         <v>467</v>
@@ -5868,7 +5908,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>972</v>
+        <v>962</v>
       </c>
       <c r="B10" t="s">
         <v>468</v>
@@ -5879,7 +5919,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>973</v>
+        <v>963</v>
       </c>
       <c r="B11" t="s">
         <v>469</v>
@@ -5890,7 +5930,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>974</v>
+        <v>964</v>
       </c>
       <c r="B12" t="s">
         <v>470</v>
@@ -5901,7 +5941,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>975</v>
+        <v>965</v>
       </c>
       <c r="B13" t="s">
         <v>471</v>
@@ -5912,7 +5952,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>976</v>
+        <v>966</v>
       </c>
       <c r="B14" t="s">
         <v>472</v>
@@ -5923,7 +5963,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>977</v>
+        <v>967</v>
       </c>
       <c r="B15" t="s">
         <v>473</v>
@@ -5934,7 +5974,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>978</v>
+        <v>968</v>
       </c>
       <c r="B16" t="s">
         <v>474</v>
@@ -5996,8 +6036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6009,7 +6049,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1008</v>
+        <v>998</v>
       </c>
       <c r="B1" t="s">
         <v>491</v>
@@ -6020,7 +6060,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>979</v>
+        <v>969</v>
       </c>
       <c r="B2" t="s">
         <v>492</v>
@@ -6031,7 +6071,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>980</v>
+        <v>970</v>
       </c>
       <c r="B3" t="s">
         <v>493</v>
@@ -6042,7 +6082,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>981</v>
+        <v>971</v>
       </c>
       <c r="B4" t="s">
         <v>494</v>
@@ -6053,7 +6093,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>982</v>
+        <v>972</v>
       </c>
       <c r="B5" t="s">
         <v>495</v>
@@ -6064,7 +6104,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>983</v>
+        <v>973</v>
       </c>
       <c r="B6" t="s">
         <v>496</v>
@@ -6075,7 +6115,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>984</v>
+        <v>974</v>
       </c>
       <c r="B7" t="s">
         <v>497</v>
@@ -6097,7 +6137,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>942</v>
+        <v>932</v>
       </c>
       <c r="B9" t="s">
         <v>499</v>
@@ -6108,7 +6148,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>985</v>
+        <v>975</v>
       </c>
       <c r="B10" t="s">
         <v>498</v>
@@ -6160,7 +6200,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>986</v>
+        <v>976</v>
       </c>
       <c r="B2" t="s">
         <v>508</v>
@@ -6171,7 +6211,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>987</v>
+        <v>977</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -6182,7 +6222,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>988</v>
+        <v>978</v>
       </c>
       <c r="B4" t="s">
         <v>509</v>
@@ -6193,7 +6233,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>989</v>
+        <v>979</v>
       </c>
       <c r="B5" t="s">
         <v>510</v>
@@ -6204,7 +6244,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>990</v>
+        <v>980</v>
       </c>
       <c r="B6" t="s">
         <v>511</v>
@@ -6215,7 +6255,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>991</v>
+        <v>981</v>
       </c>
       <c r="B7" t="s">
         <v>512</v>
@@ -6226,18 +6266,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>992</v>
+        <v>982</v>
       </c>
       <c r="B8" t="s">
         <v>513</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>993</v>
+        <v>983</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>994</v>
+        <v>984</v>
       </c>
       <c r="B9" t="s">
         <v>514</v>
@@ -6248,7 +6288,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>995</v>
+        <v>985</v>
       </c>
       <c r="B10" t="s">
         <v>515</v>
@@ -6259,7 +6299,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>996</v>
+        <v>986</v>
       </c>
       <c r="B11" t="s">
         <v>516</v>
@@ -6270,7 +6310,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>997</v>
+        <v>987</v>
       </c>
       <c r="B12" t="s">
         <v>517</v>
@@ -6281,7 +6321,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>998</v>
+        <v>988</v>
       </c>
       <c r="B13" t="s">
         <v>517</v>
@@ -6292,7 +6332,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>999</v>
+        <v>989</v>
       </c>
       <c r="B14" t="s">
         <v>518</v>
@@ -6303,7 +6343,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>1000</v>
+        <v>990</v>
       </c>
       <c r="B15" t="s">
         <v>519</v>
@@ -6314,29 +6354,29 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1001</v>
+        <v>991</v>
       </c>
       <c r="B16" t="s">
         <v>520</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>1002</v>
+        <v>992</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>986</v>
+        <v>976</v>
       </c>
       <c r="B17" t="s">
         <v>508</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>1003</v>
+        <v>993</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>1004</v>
+        <v>994</v>
       </c>
       <c r="B18" t="s">
         <v>521</v>
@@ -6347,7 +6387,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>1005</v>
+        <v>995</v>
       </c>
       <c r="B19" t="s">
         <v>522</v>
@@ -6358,7 +6398,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>1006</v>
+        <v>996</v>
       </c>
       <c r="B20" t="s">
         <v>523</v>
@@ -6369,7 +6409,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>1007</v>
+        <v>997</v>
       </c>
       <c r="B21" t="s">
         <v>524</v>
@@ -6380,7 +6420,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>941</v>
+        <v>931</v>
       </c>
       <c r="B22" t="s">
         <v>396</v>
@@ -6391,7 +6431,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>942</v>
+        <v>932</v>
       </c>
       <c r="B23" t="s">
         <v>152</v>
@@ -6402,7 +6442,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>985</v>
+        <v>975</v>
       </c>
       <c r="B24" t="s">
         <v>154</v>
@@ -6413,7 +6453,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>943</v>
+        <v>933</v>
       </c>
       <c r="B25" t="s">
         <v>397</v>
@@ -9027,7 +9067,7 @@
       <c r="AT14"/>
       <c r="AU14"/>
     </row>
-    <row r="15" spans="1:47" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>765</v>
       </c>
@@ -9409,8 +9449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9743,7 +9783,7 @@
     </row>
     <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>816</v>
+        <v>1008</v>
       </c>
       <c r="B30" t="s">
         <v>132</v>
@@ -9754,7 +9794,7 @@
     </row>
     <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>817</v>
+        <v>999</v>
       </c>
       <c r="B31" t="s">
         <v>133</v>
@@ -9765,7 +9805,7 @@
     </row>
     <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>818</v>
+        <v>1000</v>
       </c>
       <c r="B32" t="s">
         <v>134</v>
@@ -9776,7 +9816,7 @@
     </row>
     <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>819</v>
+        <v>1001</v>
       </c>
       <c r="B33" t="s">
         <v>135</v>
@@ -9787,7 +9827,7 @@
     </row>
     <row r="34" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>820</v>
+        <v>1002</v>
       </c>
       <c r="B34" t="s">
         <v>136</v>
@@ -9798,7 +9838,7 @@
     </row>
     <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>821</v>
+        <v>1003</v>
       </c>
       <c r="B35" t="s">
         <v>137</v>
@@ -9809,7 +9849,7 @@
     </row>
     <row r="36" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>822</v>
+        <v>1004</v>
       </c>
       <c r="B36" t="s">
         <v>138</v>
@@ -9820,7 +9860,7 @@
     </row>
     <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>823</v>
+        <v>1005</v>
       </c>
       <c r="B37" t="s">
         <v>139</v>
@@ -9831,7 +9871,7 @@
     </row>
     <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>824</v>
+        <v>1006</v>
       </c>
       <c r="B38" t="s">
         <v>140</v>
@@ -9842,7 +9882,7 @@
     </row>
     <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>825</v>
+        <v>1007</v>
       </c>
       <c r="B39" t="s">
         <v>141</v>
@@ -9853,7 +9893,7 @@
     </row>
     <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>826</v>
+        <v>816</v>
       </c>
       <c r="B40" t="s">
         <v>142</v>
@@ -9864,7 +9904,7 @@
     </row>
     <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>827</v>
+        <v>817</v>
       </c>
       <c r="B41" t="s">
         <v>143</v>
@@ -9875,7 +9915,7 @@
     </row>
     <row r="42" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>828</v>
+        <v>818</v>
       </c>
       <c r="B42" t="s">
         <v>144</v>
@@ -9886,7 +9926,7 @@
     </row>
     <row r="43" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>829</v>
+        <v>819</v>
       </c>
       <c r="B43" t="s">
         <v>145</v>
@@ -9897,7 +9937,7 @@
     </row>
     <row r="44" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>830</v>
+        <v>820</v>
       </c>
       <c r="B44" t="s">
         <v>146</v>
@@ -9908,7 +9948,7 @@
     </row>
     <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>831</v>
+        <v>821</v>
       </c>
       <c r="B45" t="s">
         <v>147</v>
@@ -9919,7 +9959,7 @@
     </row>
     <row r="46" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>832</v>
+        <v>822</v>
       </c>
       <c r="B46" t="s">
         <v>148</v>
@@ -9930,7 +9970,7 @@
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>833</v>
+        <v>823</v>
       </c>
       <c r="B47" t="s">
         <v>149</v>
@@ -9941,7 +9981,7 @@
     </row>
     <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>832</v>
+        <v>822</v>
       </c>
       <c r="B48" t="s">
         <v>148</v>
@@ -9952,18 +9992,18 @@
     </row>
     <row r="49" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="B49" t="s">
         <v>150</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>835</v>
+        <v>825</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>836</v>
+        <v>826</v>
       </c>
       <c r="B50" t="s">
         <v>151</v>
@@ -10048,7 +10088,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>837</v>
+        <v>827</v>
       </c>
       <c r="B1" t="s">
         <v>208</v>
@@ -10059,7 +10099,7 @@
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>838</v>
+        <v>828</v>
       </c>
       <c r="B2" t="s">
         <v>209</v>
@@ -10070,7 +10110,7 @@
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>839</v>
+        <v>829</v>
       </c>
       <c r="B3" t="s">
         <v>210</v>
@@ -10081,7 +10121,7 @@
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>840</v>
+        <v>830</v>
       </c>
       <c r="B4" t="s">
         <v>211</v>
@@ -10092,7 +10132,7 @@
     </row>
     <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>841</v>
+        <v>831</v>
       </c>
       <c r="B5" t="s">
         <v>212</v>
@@ -10103,7 +10143,7 @@
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>842</v>
+        <v>832</v>
       </c>
       <c r="B6" t="s">
         <v>213</v>
@@ -10114,7 +10154,7 @@
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>843</v>
+        <v>833</v>
       </c>
       <c r="B7" t="s">
         <v>214</v>
@@ -10125,7 +10165,7 @@
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="B8" t="s">
         <v>215</v>
@@ -10136,7 +10176,7 @@
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="B9" t="s">
         <v>216</v>
@@ -10147,7 +10187,7 @@
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>846</v>
+        <v>836</v>
       </c>
       <c r="B10" t="s">
         <v>217</v>
@@ -10158,7 +10198,7 @@
     </row>
     <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="B11" t="s">
         <v>218</v>
@@ -10169,7 +10209,7 @@
     </row>
     <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>848</v>
+        <v>838</v>
       </c>
       <c r="B12" t="s">
         <v>219</v>
@@ -10180,7 +10220,7 @@
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>849</v>
+        <v>839</v>
       </c>
       <c r="B13" t="s">
         <v>220</v>
@@ -10191,7 +10231,7 @@
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>850</v>
+        <v>840</v>
       </c>
       <c r="B14" t="s">
         <v>221</v>
@@ -10202,7 +10242,7 @@
     </row>
     <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>851</v>
+        <v>841</v>
       </c>
       <c r="B15" t="s">
         <v>222</v>
@@ -10213,7 +10253,7 @@
     </row>
     <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>852</v>
+        <v>842</v>
       </c>
       <c r="B16" t="s">
         <v>223</v>
@@ -10224,7 +10264,7 @@
     </row>
     <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>853</v>
+        <v>843</v>
       </c>
       <c r="B17" t="s">
         <v>209</v>

</xml_diff>